<commit_message>
[harshada]: New testcase added for home page filter dropdown
</commit_message>
<xml_diff>
--- a/Test data/Swag Lab Test Data.xlsx
+++ b/Test data/Swag Lab Test Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sairam\eclipse-workspace\SwagLab\Test data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8E695C-8C21-4203-97D3-4BBBF08982EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4181ADAD-057F-4AF6-B138-E2CC6C30913F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3375" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{9464BE0B-845B-40FE-ADDD-3A41F45C3D05}"/>
   </bookViews>
@@ -35,25 +35,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>https://www.saucedemo.com/inventory.html</t>
   </si>
   <si>
     <t>REMOVE</t>
+  </si>
+  <si>
+    <t>Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>Sauce Labs Onesie</t>
+  </si>
+  <si>
+    <t>Sauce Labs Fleece Jacket</t>
+  </si>
+  <si>
+    <t>Price (low to high)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,28 +410,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DB3C40-A42A-464A-BE07-73FD676D5D40}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>